<commit_message>
Add himki, add rule to all
</commit_message>
<xml_diff>
--- a/xlsx/cheboksari.xlsx
+++ b/xlsx/cheboksari.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,7 +461,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>109</t>
+          <t>110</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -471,63 +471,63 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>X50</t>
+          <t>X70</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>2590190</v>
+        <v>2946190</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19106.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20281.html</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>2590190</v>
+        <v>2946190</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19106.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20281.html</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>110</t>
+          <t>119</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Belgee</t>
+          <t>Changan</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>X70</t>
+          <t>Alsvin</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2946190</v>
+        <v>1899900</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_20281.html</t>
+          <t>https://alyans-auto.ru/auto/auto_17047.html</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>2946190</v>
+        <v>1899900</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_20281.html</t>
+          <t>https://alyans-auto.ru/auto/auto_17047.html</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>119</t>
+          <t>115</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -537,30 +537,30 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Alsvin</t>
+          <t>CS35 Plus</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1899900</v>
+        <v>2629900</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_17047.html</t>
+          <t>https://alyans-auto.ru/auto/auto_18452.html</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>1899900</v>
+        <v>2629900</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_17047.html</t>
+          <t>https://alyans-auto.ru/auto/auto_18452.html</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>115</t>
+          <t>135</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -570,30 +570,30 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>CS35 Plus</t>
+          <t>CS75 Plus</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>2629900</v>
+        <v>3949900</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_18452.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20246.html</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>2629900</v>
+        <v>3949900</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_18452.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20246.html</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>135</t>
+          <t>125</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -603,30 +603,30 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>CS75 Plus</t>
+          <t>CS95</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>3949900</v>
+        <v>4609900</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_20246.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19734.html</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>3949900</v>
+        <v>4609900</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_20246.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19734.html</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>125</t>
+          <t>128</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -636,30 +636,30 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>CS95</t>
+          <t>Eado Plus</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>4609900</v>
+        <v>2529900</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19734.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19163.html</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>4609900</v>
+        <v>2529900</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19734.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19163.html</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>128</t>
+          <t>120</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -669,30 +669,30 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Eado Plus</t>
+          <t>UNI-K</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>2529900</v>
+        <v>4549900</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19163.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20242.html</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>2529900</v>
+        <v>4549900</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19163.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20242.html</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>141</t>
+          <t>127</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -702,30 +702,30 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Hunter Plus</t>
+          <t>UNI-S</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>3739900</v>
+        <v>2959900</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_18934.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19722.html</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>3739900</v>
+        <v>2959900</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_18934.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19722.html</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>126</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -735,30 +735,30 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>UNI-K</t>
+          <t>UNI-T</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>4549900</v>
+        <v>3239900</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_20241.html</t>
+          <t>https://alyans-auto.ru/auto/auto_17449.html</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>4549900</v>
+        <v>3239900</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_20241.html</t>
+          <t>https://alyans-auto.ru/auto/auto_17449.html</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>127</t>
+          <t>123</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -768,96 +768,96 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>UNI-S</t>
+          <t>UNI-V</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>2959900</v>
+        <v>3209900</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19724.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19626.html</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>2959900</v>
+        <v>3209900</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19724.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19626.html</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>126</t>
+          <t>251</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Changan</t>
+          <t>Geely</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>UNI-T</t>
+          <t>Atlas New</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>3239900</v>
+        <v>3817190</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_17449.html</t>
+          <t>https://alyans-auto.ru/auto/auto_17856.html</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>3239900</v>
+        <v>3817190</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_17449.html</t>
+          <t>https://alyans-auto.ru/auto/auto_17856.html</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>123</t>
+          <t>772</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Changan</t>
+          <t>Geely</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>UNI-V</t>
+          <t>Cityray</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>3209900</v>
+        <v>3214190</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19626.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19834.html</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>3209900</v>
+        <v>3214190</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19626.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19834.html</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>251</t>
+          <t>255</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -867,30 +867,30 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Atlas New</t>
+          <t>Coolray</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>3717190</v>
+        <v>2799190</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_17846.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19201.html</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>3717190</v>
+        <v>2799190</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_17846.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19201.html</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>772</t>
+          <t>260</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -900,30 +900,30 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Cityray</t>
+          <t>Emgrand</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>3214190</v>
+        <v>2243990</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19834.html</t>
+          <t>https://alyans-auto.ru/auto/auto_18246.html</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>3214190</v>
+        <v>2243990</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19834.html</t>
+          <t>https://alyans-auto.ru/auto/auto_18246.html</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>255</t>
+          <t>265</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -933,30 +933,30 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Coolray</t>
+          <t>Monjaro</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>2799190</v>
+        <v>4552190</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19201.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20005.html</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>2799190</v>
+        <v>4552190</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19201.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20005.html</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>260</t>
+          <t>267</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -966,30 +966,30 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Emgrand</t>
+          <t>Okavango</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2243990</v>
+        <v>3697190</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_18246.html</t>
+          <t>https://alyans-auto.ru/auto/auto_17103.html</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>2243990</v>
+        <v>3697190</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_18246.html</t>
+          <t>https://alyans-auto.ru/auto/auto_17103.html</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>265</t>
+          <t>773</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -999,129 +999,129 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Monjaro</t>
+          <t>Preface FS11</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>4552190</v>
+        <v>3359190</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_20005.html</t>
+          <t>https://alyans-auto.ru/auto/auto_18229.html</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>4552190</v>
+        <v>3359190</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_20005.html</t>
+          <t>https://alyans-auto.ru/auto/auto_18229.html</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>267</t>
+          <t>273</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Geely</t>
+          <t>Great Wall</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Okavango</t>
+          <t>POER</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>3697190</v>
+        <v>3499000</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_17103.html</t>
+          <t>https://alyans-auto.ru/auto/auto_13123.html</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>3697190</v>
+        <v>3499000</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_17103.html</t>
+          <t>https://alyans-auto.ru/auto/auto_13123.html</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>773</t>
+          <t>286</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Geely</t>
+          <t>Haval</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Preface FS11</t>
+          <t>Dargo</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>3359190</v>
+        <v>3349000</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_18229.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20092.html</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>3359190</v>
+        <v>3349000</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_18229.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20092.html</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>273</t>
+          <t>304</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Great Wall</t>
+          <t>Haval</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>POER</t>
+          <t>F7</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>3499000</v>
+        <v>3049000</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_13123.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20288.html</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>3499000</v>
+        <v>3049000</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_13123.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20288.html</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>286</t>
+          <t>301</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1131,30 +1131,30 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Dargo</t>
+          <t>Jolion</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>3349000</v>
+        <v>2149000</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_20092.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20109.html</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>3349000</v>
+        <v>2149000</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_20092.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20109.html</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>304</t>
+          <t>307</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1164,96 +1164,96 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>F7</t>
+          <t>M6</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>2849000</v>
+        <v>2179000</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19865.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20009.html</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>2849000</v>
+        <v>2179000</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19865.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20009.html</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>301</t>
+          <t>337</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Haval</t>
+          <t>JAC</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Jolion</t>
+          <t>J7</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>2049000</v>
+        <v>2149000</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19277.html</t>
+          <t>https://alyans-auto.ru/auto/auto_15496.html</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>2049000</v>
+        <v>2149000</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19277.html</t>
+          <t>https://alyans-auto.ru/auto/auto_15496.html</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>307</t>
+          <t>338</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Haval</t>
+          <t>JAC</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>M6</t>
+          <t>JS3</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>2179000</v>
+        <v>1889000</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19966.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19964.html</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>2179000</v>
+        <v>1889000</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19966.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19964.html</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>337</t>
+          <t>340</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1263,30 +1263,30 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>J7</t>
+          <t>JS6</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>2149000</v>
+        <v>2809000</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_15496.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19965.html</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>2149000</v>
+        <v>2809000</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_15496.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19965.html</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>338</t>
+          <t>344</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1296,30 +1296,30 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>JS3</t>
+          <t>T6</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>1889000</v>
+        <v>2665500</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19964.html</t>
+          <t>https://alyans-auto.ru/auto/auto_8942.html</t>
         </is>
       </c>
       <c r="F27" t="n">
-        <v>1889000</v>
+        <v>2665500</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19964.html</t>
+          <t>https://alyans-auto.ru/auto/auto_8942.html</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>340</t>
+          <t>681</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1329,30 +1329,30 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>JS6</t>
+          <t>T8</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>2399000</v>
+        <v>3259000</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_13473.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19960.html</t>
         </is>
       </c>
       <c r="F28" t="n">
-        <v>2399000</v>
+        <v>3259000</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_13473.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19960.html</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>344</t>
+          <t>345</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1362,30 +1362,30 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>T6</t>
+          <t>T8 Pro</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>2665500</v>
+        <v>3279000</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_8942.html</t>
+          <t>https://alyans-auto.ru/auto/auto_18038.html</t>
         </is>
       </c>
       <c r="F29" t="n">
-        <v>2665500</v>
+        <v>3279000</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_8942.html</t>
+          <t>https://alyans-auto.ru/auto/auto_18038.html</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>681</t>
+          <t>682</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1395,195 +1395,195 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>T8</t>
+          <t>T9</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>3259000</v>
+        <v>3599000</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19960.html</t>
+          <t>https://alyans-auto.ru/auto/auto_18643.html</t>
         </is>
       </c>
       <c r="F30" t="n">
-        <v>3259000</v>
+        <v>3599000</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19960.html</t>
+          <t>https://alyans-auto.ru/auto/auto_18643.html</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>345</t>
+          <t>347</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>JAC</t>
+          <t>JAECOO</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>T8 Pro</t>
+          <t>J7</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>3279000</v>
+        <v>2339900</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_18038.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20256.html</t>
         </is>
       </c>
       <c r="F31" t="n">
-        <v>3279000</v>
+        <v>2339900</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_18038.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20256.html</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>682</t>
+          <t>348</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>JAC</t>
+          <t>JAECOO</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>T9</t>
+          <t>J8</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>3599000</v>
+        <v>4349000</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_18643.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20253.html</t>
         </is>
       </c>
       <c r="F32" t="n">
-        <v>3599000</v>
+        <v>4349000</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_18643.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20253.html</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>347</t>
+          <t>775</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>JAECOO</t>
+          <t>Knewstar</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>J7</t>
+          <t>001</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>2339900</v>
+        <v>4393190</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_20256.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19305.html</t>
         </is>
       </c>
       <c r="F33" t="n">
-        <v>2339900</v>
+        <v>4393190</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_20256.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19305.html</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>348</t>
+          <t>701</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>JAECOO</t>
+          <t>Lada</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>J8</t>
+          <t>4x4 3 двери</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>4349000</v>
+        <v>1059000</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_20100.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19270.html</t>
         </is>
       </c>
       <c r="F34" t="n">
-        <v>4349000</v>
+        <v>1059000</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_20100.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19270.html</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>775</t>
+          <t>406</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Knewstar</t>
+          <t>Lada</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>001</t>
+          <t>Granta Sedan</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>4393190</v>
+        <v>1043500</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19305.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19756.html</t>
         </is>
       </c>
       <c r="F35" t="n">
-        <v>4393190</v>
+        <v>1043500</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19305.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19756.html</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>701</t>
+          <t>418</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1593,30 +1593,30 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>4x4 3 двери</t>
+          <t>Largus</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>1059000</v>
+        <v>1670000</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19270.html</t>
+          <t>https://alyans-auto.ru/auto/auto_16658.html</t>
         </is>
       </c>
       <c r="F36" t="n">
-        <v>1059000</v>
+        <v>1670000</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19270.html</t>
+          <t>https://alyans-auto.ru/auto/auto_16658.html</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>406</t>
+          <t>422</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1626,30 +1626,30 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Granta Sedan</t>
+          <t>Niva</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>1038500</v>
+        <v>1310500</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_17756.html</t>
+          <t>https://alyans-auto.ru/auto/auto_14903.html</t>
         </is>
       </c>
       <c r="F37" t="n">
-        <v>1038500</v>
+        <v>1310500</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_17756.html</t>
+          <t>https://alyans-auto.ru/auto/auto_14903.html</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>418</t>
+          <t>435</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1659,30 +1659,30 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Largus</t>
+          <t>Vesta Sedan</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>1670000</v>
+        <v>1586500</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_16658.html</t>
+          <t>https://alyans-auto.ru/auto/auto_13028.html</t>
         </is>
       </c>
       <c r="F38" t="n">
-        <v>1670000</v>
+        <v>1586500</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_16658.html</t>
+          <t>https://alyans-auto.ru/auto/auto_13028.html</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>422</t>
+          <t>784</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1692,30 +1692,30 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Niva</t>
+          <t>ВИС 2346</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>1310500</v>
+        <v>1511000</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_14903.html</t>
+          <t>https://alyans-auto.ru/auto/auto_18062.html</t>
         </is>
       </c>
       <c r="F39" t="n">
-        <v>1310500</v>
+        <v>1511000</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_14903.html</t>
+          <t>https://alyans-auto.ru/auto/auto_18062.html</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>435</t>
+          <t>859</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1725,221 +1725,155 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Vesta Sedan</t>
+          <t>ВИС 2349 Пикап</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>1586500</v>
+        <v>1364100</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_13028.html</t>
+          <t>https://alyans-auto.ru/auto/auto_14192.html</t>
         </is>
       </c>
       <c r="F40" t="n">
-        <v>1586500</v>
+        <v>1364100</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_13028.html</t>
+          <t>https://alyans-auto.ru/auto/auto_14192.html</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>784</t>
+          <t>525</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Lada</t>
+          <t>OMODA</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>ВИС 2346</t>
+          <t>C5</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>1511000</v>
+        <v>1889900</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_18062.html</t>
+          <t>https://alyans-auto.ru/auto/auto_17980.html</t>
         </is>
       </c>
       <c r="F41" t="n">
-        <v>1511000</v>
+        <v>1889900</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_18062.html</t>
+          <t>https://alyans-auto.ru/auto/auto_17980.html</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>859</t>
+          <t>526</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Lada</t>
+          <t>OMODA</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>ВИС 2349 Пикап</t>
+          <t>S5</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>1364100</v>
+        <v>1809900</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_14192.html</t>
+          <t>https://alyans-auto.ru/auto/auto_16128.html</t>
         </is>
       </c>
       <c r="F42" t="n">
-        <v>1364100</v>
+        <v>1809900</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_14192.html</t>
+          <t>https://alyans-auto.ru/auto/auto_16128.html</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>525</t>
+          <t>675</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>OMODA</t>
+          <t>XCite</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>C5</t>
+          <t>X-Cross 7</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>1889900</v>
+        <v>2495500</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_17980.html</t>
+          <t>https://alyans-auto.ru/auto/auto_17597.html</t>
         </is>
       </c>
       <c r="F43" t="n">
-        <v>1889900</v>
+        <v>2495500</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_17980.html</t>
+          <t>https://alyans-auto.ru/auto/auto_17597.html</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>526</t>
+          <t>787</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>OMODA</t>
+          <t>XCite</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>S5</t>
+          <t>X-Cross 8</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>1809900</v>
+        <v>2999000</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_16128.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19840.html</t>
         </is>
       </c>
       <c r="F44" t="n">
-        <v>1809900</v>
+        <v>2999000</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_16128.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>675</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>XCite</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>X-Cross 7</t>
-        </is>
-      </c>
-      <c r="D45" t="n">
-        <v>2495500</v>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>https://alyans-auto.ru/auto/auto_17597.html</t>
-        </is>
-      </c>
-      <c r="F45" t="n">
-        <v>2495500</v>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>https://alyans-auto.ru/auto/auto_17597.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>787</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>XCite</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>X-Cross 8</t>
-        </is>
-      </c>
-      <c r="D46" t="n">
-        <v>2999000</v>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>https://alyans-auto.ru/auto/auto_18333.html</t>
-        </is>
-      </c>
-      <c r="F46" t="n">
-        <v>2999000</v>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>https://alyans-auto.ru/auto/auto_18333.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19840.html</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix che, omsk, krd
</commit_message>
<xml_diff>
--- a/xlsx/cheboksari.xlsx
+++ b/xlsx/cheboksari.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -593,7 +593,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>125</t>
+          <t>128</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -603,30 +603,30 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>CS95</t>
+          <t>Eado Plus</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>4609900</v>
+        <v>2529900</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19734.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19163.html</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>4609900</v>
+        <v>2529900</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19734.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19163.html</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>128</t>
+          <t>120</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -636,30 +636,30 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Eado Plus</t>
+          <t>UNI-K</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>2529900</v>
+        <v>5219900</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19163.html</t>
+          <t>https://alyans-auto.ru/auto/auto_10350.html</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>2529900</v>
+        <v>5219900</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19163.html</t>
+          <t>https://alyans-auto.ru/auto/auto_10350.html</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>127</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -669,30 +669,30 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>UNI-K</t>
+          <t>UNI-S</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>5219900</v>
+        <v>2959900</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_10350.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20044.html</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>5219900</v>
+        <v>2959900</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_10350.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20044.html</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>127</t>
+          <t>126</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -702,96 +702,96 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>UNI-S</t>
+          <t>UNI-T</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2959900</v>
+        <v>3239900</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19901.html</t>
+          <t>https://alyans-auto.ru/auto/auto_17449.html</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>2959900</v>
+        <v>3239900</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19901.html</t>
+          <t>https://alyans-auto.ru/auto/auto_17449.html</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>126</t>
+          <t>251</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Changan</t>
+          <t>Geely</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>UNI-T</t>
+          <t>Atlas New</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>3239900</v>
+        <v>3817990</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_17449.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19129.html</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>3239900</v>
+        <v>3817990</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_17449.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19129.html</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>123</t>
+          <t>772</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Changan</t>
+          <t>Geely</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>UNI-V</t>
+          <t>Cityray</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>3209900</v>
+        <v>3094190</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19627.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19832.html</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>3209900</v>
+        <v>3094190</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19627.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19832.html</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>251</t>
+          <t>255</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -801,30 +801,30 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Atlas New</t>
+          <t>Coolray</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>3817190</v>
+        <v>2799190</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_17856.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19201.html</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>3817190</v>
+        <v>2799190</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_17856.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19201.html</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>772</t>
+          <t>260</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -834,30 +834,30 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Cityray</t>
+          <t>Emgrand</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>3214190</v>
+        <v>2393990</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19834.html</t>
+          <t>https://alyans-auto.ru/auto/auto_17740.html</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>3214190</v>
+        <v>2393990</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19834.html</t>
+          <t>https://alyans-auto.ru/auto/auto_17740.html</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>255</t>
+          <t>265</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -867,30 +867,30 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Coolray</t>
+          <t>Monjaro</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>2799190</v>
+        <v>4552190</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19201.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20005.html</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>2799190</v>
+        <v>4552190</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19201.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20005.html</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>260</t>
+          <t>267</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -900,30 +900,30 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Emgrand</t>
+          <t>Okavango</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>2243990</v>
+        <v>3697190</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_18246.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20015.html</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>2243990</v>
+        <v>3697190</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_18246.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20015.html</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>265</t>
+          <t>773</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -933,129 +933,129 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Monjaro</t>
+          <t>Preface FS11</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>4552190</v>
+        <v>3359190</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_20005.html</t>
+          <t>https://alyans-auto.ru/auto/auto_18229.html</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>4552190</v>
+        <v>3359190</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_20005.html</t>
+          <t>https://alyans-auto.ru/auto/auto_18229.html</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>267</t>
+          <t>273</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Geely</t>
+          <t>Great Wall</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Okavango</t>
+          <t>POER</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>3697190</v>
+        <v>3499000</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_20015.html</t>
+          <t>https://alyans-auto.ru/auto/auto_13123.html</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>3697190</v>
+        <v>3499000</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_20015.html</t>
+          <t>https://alyans-auto.ru/auto/auto_13123.html</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>773</t>
+          <t>286</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Geely</t>
+          <t>Haval</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Preface FS11</t>
+          <t>Dargo</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>3359190</v>
+        <v>3349000</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_18229.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20621.html</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>3359190</v>
+        <v>3349000</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_18229.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20621.html</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>273</t>
+          <t>304</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Great Wall</t>
+          <t>Haval</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>POER</t>
+          <t>F7</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>3499000</v>
+        <v>3049000</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_13123.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20428.html</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>3499000</v>
+        <v>3049000</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_13123.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20428.html</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>286</t>
+          <t>301</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1065,30 +1065,30 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Dargo</t>
+          <t>Jolion</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>3349000</v>
+        <v>2149000</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_20092.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20287.html</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>3349000</v>
+        <v>2149000</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_20092.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20287.html</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>304</t>
+          <t>307</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1098,40 +1098,40 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>F7</t>
+          <t>M6</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>3049000</v>
+        <v>2179000</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_20288.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20592.html</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>3049000</v>
+        <v>2179000</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_20288.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20592.html</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>301</t>
+          <t>337</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Haval</t>
+          <t>JAC</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Jolion</t>
+          <t>J7</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -1139,7 +1139,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_20287.html</t>
+          <t>https://alyans-auto.ru/auto/auto_15496.html</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -1147,47 +1147,47 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_20287.html</t>
+          <t>https://alyans-auto.ru/auto/auto_15496.html</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>307</t>
+          <t>338</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Haval</t>
+          <t>JAC</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>M6</t>
+          <t>JS3</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>2179000</v>
+        <v>1889000</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_20480.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19964.html</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>2179000</v>
+        <v>1889000</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_20480.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19964.html</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>337</t>
+          <t>340</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1197,30 +1197,30 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>J7</t>
+          <t>JS6</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>2149000</v>
+        <v>2809000</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_15496.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19965.html</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>2149000</v>
+        <v>2809000</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_15496.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19965.html</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>338</t>
+          <t>344</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1230,30 +1230,30 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>JS3</t>
+          <t>T6</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>1889000</v>
+        <v>2665500</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19964.html</t>
+          <t>https://alyans-auto.ru/auto/auto_8942.html</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>1889000</v>
+        <v>2665500</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19964.html</t>
+          <t>https://alyans-auto.ru/auto/auto_8942.html</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>340</t>
+          <t>681</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1263,30 +1263,30 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>JS6</t>
+          <t>T8</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>2809000</v>
+        <v>3259000</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19965.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19960.html</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>2809000</v>
+        <v>3259000</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19965.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19960.html</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>344</t>
+          <t>345</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1296,228 +1296,228 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>T6</t>
+          <t>T8 Pro</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>2665500</v>
+        <v>3279000</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_8942.html</t>
+          <t>https://alyans-auto.ru/auto/auto_18038.html</t>
         </is>
       </c>
       <c r="F27" t="n">
-        <v>2665500</v>
+        <v>3279000</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_8942.html</t>
+          <t>https://alyans-auto.ru/auto/auto_18038.html</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>681</t>
+          <t>347</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>JAC</t>
+          <t>JAECOO</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>T8</t>
+          <t>J7</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>3259000</v>
+        <v>2699900</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19960.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19844.html</t>
         </is>
       </c>
       <c r="F28" t="n">
-        <v>3259000</v>
+        <v>2699900</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19960.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19844.html</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>345</t>
+          <t>348</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>JAC</t>
+          <t>JAECOO</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>T8 Pro</t>
+          <t>J8</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>3279000</v>
+        <v>4349000</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_18038.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20253.html</t>
         </is>
       </c>
       <c r="F29" t="n">
-        <v>3279000</v>
+        <v>4349000</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_18038.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20253.html</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>682</t>
+          <t>775</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>JAC</t>
+          <t>Knewstar</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>T9</t>
+          <t>001</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>3599000</v>
+        <v>4393190</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_18643.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19305.html</t>
         </is>
       </c>
       <c r="F30" t="n">
-        <v>3599000</v>
+        <v>4393190</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_18643.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19305.html</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>347</t>
+          <t>701</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>JAECOO</t>
+          <t>Lada</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>J7</t>
+          <t>4x4 3 двери</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>2639900</v>
+        <v>1055500</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19844.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20482.html</t>
         </is>
       </c>
       <c r="F31" t="n">
-        <v>2639900</v>
+        <v>1055500</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19844.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20482.html</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>348</t>
+          <t>406</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>JAECOO</t>
+          <t>Lada</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>J8</t>
+          <t>Granta Sedan</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>4349000</v>
+        <v>1043500</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_20253.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19756.html</t>
         </is>
       </c>
       <c r="F32" t="n">
-        <v>4349000</v>
+        <v>1043500</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_20253.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19756.html</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>775</t>
+          <t>418</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Knewstar</t>
+          <t>Lada</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>001</t>
+          <t>Largus</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>4393190</v>
+        <v>1660000</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19305.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20549.html</t>
         </is>
       </c>
       <c r="F33" t="n">
-        <v>4393190</v>
+        <v>1660000</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19305.html</t>
+          <t>https://alyans-auto.ru/auto/auto_20549.html</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>701</t>
+          <t>422</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1527,30 +1527,30 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>4x4 3 двери</t>
+          <t>Niva</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>1055500</v>
+        <v>1310500</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_20482.html</t>
+          <t>https://alyans-auto.ru/auto/auto_14903.html</t>
         </is>
       </c>
       <c r="F34" t="n">
-        <v>1055500</v>
+        <v>1310500</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_20482.html</t>
+          <t>https://alyans-auto.ru/auto/auto_14903.html</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>406</t>
+          <t>435</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1560,30 +1560,30 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Granta Sedan</t>
+          <t>Vesta Sedan</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>1043500</v>
+        <v>1586500</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19756.html</t>
+          <t>https://alyans-auto.ru/auto/auto_13028.html</t>
         </is>
       </c>
       <c r="F35" t="n">
-        <v>1043500</v>
+        <v>1586500</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_19756.html</t>
+          <t>https://alyans-auto.ru/auto/auto_13028.html</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>418</t>
+          <t>784</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1593,30 +1593,30 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Largus</t>
+          <t>ВИС 2346</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>1670000</v>
+        <v>1511000</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_18870.html</t>
+          <t>https://alyans-auto.ru/auto/auto_18062.html</t>
         </is>
       </c>
       <c r="F36" t="n">
-        <v>1670000</v>
+        <v>1511000</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_18870.html</t>
+          <t>https://alyans-auto.ru/auto/auto_18062.html</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>422</t>
+          <t>859</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1626,252 +1626,153 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Niva</t>
+          <t>ВИС 2349 Пикап</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>1310500</v>
+        <v>1364100</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_14903.html</t>
+          <t>https://alyans-auto.ru/auto/auto_14192.html</t>
         </is>
       </c>
       <c r="F37" t="n">
-        <v>1310500</v>
+        <v>1364100</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_14903.html</t>
+          <t>https://alyans-auto.ru/auto/auto_14192.html</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>435</t>
+          <t>525</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Lada</t>
+          <t>OMODA</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Vesta Sedan</t>
+          <t>C5</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>1586500</v>
+        <v>1889900</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_13028.html</t>
+          <t>https://alyans-auto.ru/auto/auto_17980.html</t>
         </is>
       </c>
       <c r="F38" t="n">
-        <v>1586500</v>
+        <v>1889900</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_13028.html</t>
+          <t>https://alyans-auto.ru/auto/auto_17980.html</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>784</t>
+          <t>526</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Lada</t>
+          <t>OMODA</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>ВИС 2346</t>
+          <t>S5</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>1511000</v>
+        <v>1809900</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_18062.html</t>
+          <t>https://alyans-auto.ru/auto/auto_17470.html</t>
         </is>
       </c>
       <c r="F39" t="n">
-        <v>1511000</v>
+        <v>1809900</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_18062.html</t>
+          <t>https://alyans-auto.ru/auto/auto_17470.html</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>859</t>
+          <t>675</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Lada</t>
+          <t>XCite</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>ВИС 2349 Пикап</t>
+          <t>X-Cross 7</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>1364100</v>
+        <v>2495500</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_14192.html</t>
+          <t>https://alyans-auto.ru/auto/auto_17597.html</t>
         </is>
       </c>
       <c r="F40" t="n">
-        <v>1364100</v>
+        <v>2495500</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_14192.html</t>
+          <t>https://alyans-auto.ru/auto/auto_17597.html</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>525</t>
+          <t>787</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>OMODA</t>
+          <t>XCite</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>C5</t>
+          <t>X-Cross 8</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>1889900</v>
+        <v>2999000</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>https://alyans-auto.ru/auto/auto_17980.html</t>
+          <t>https://alyans-auto.ru/auto/auto_19840.html</t>
         </is>
       </c>
       <c r="F41" t="n">
-        <v>1889900</v>
+        <v>2999000</v>
       </c>
       <c r="G41" t="inlineStr">
-        <is>
-          <t>https://alyans-auto.ru/auto/auto_17980.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>526</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>OMODA</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>S5</t>
-        </is>
-      </c>
-      <c r="D42" t="n">
-        <v>1809900</v>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>https://alyans-auto.ru/auto/auto_16128.html</t>
-        </is>
-      </c>
-      <c r="F42" t="n">
-        <v>1809900</v>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>https://alyans-auto.ru/auto/auto_16128.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>675</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>XCite</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>X-Cross 7</t>
-        </is>
-      </c>
-      <c r="D43" t="n">
-        <v>2495500</v>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>https://alyans-auto.ru/auto/auto_17597.html</t>
-        </is>
-      </c>
-      <c r="F43" t="n">
-        <v>2495500</v>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>https://alyans-auto.ru/auto/auto_17597.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>787</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>XCite</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>X-Cross 8</t>
-        </is>
-      </c>
-      <c r="D44" t="n">
-        <v>2999000</v>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>https://alyans-auto.ru/auto/auto_19840.html</t>
-        </is>
-      </c>
-      <c r="F44" t="n">
-        <v>2999000</v>
-      </c>
-      <c r="G44" t="inlineStr">
         <is>
           <t>https://alyans-auto.ru/auto/auto_19840.html</t>
         </is>

</xml_diff>